<commit_message>
Updated to reference data
</commit_message>
<xml_diff>
--- a/tabular/reference-set-data.xlsx
+++ b/tabular/reference-set-data.xlsx
@@ -4249,8 +4249,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="683">
+  <cellStyleXfs count="685">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4987,7 +4989,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="683">
+  <cellStyles count="685">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5329,6 +5331,7 @@
     <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5670,6 +5673,7 @@
     <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6002,7 +6006,7 @@
   <dimension ref="A1:M514"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B15" sqref="A1:M514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25556,7 +25560,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K222 K224 K226">
+  <conditionalFormatting sqref="K224 K222 K226">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
various updates aimed at generating / importing the reference phylogeny.
</commit_message>
<xml_diff>
--- a/tabular/reference-set-data.xlsx
+++ b/tabular/reference-set-data.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshsinger/gitrepos_ssh/RABV-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13760" yWindow="1460" windowWidth="32140" windowHeight="25140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5512" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5512" uniqueCount="1364">
   <si>
     <t>Accession</t>
   </si>
@@ -4102,6 +4110,15 @@
   </si>
   <si>
     <t>Minor_clade</t>
+  </si>
+  <si>
+    <t>AM2b</t>
+  </si>
+  <si>
+    <t>AM4</t>
+  </si>
+  <si>
+    <t>MYu</t>
   </si>
 </sst>
 </file>
@@ -4936,7 +4953,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4986,6 +5003,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5678,6 +5698,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -6005,11 +6030,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M514"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:M514"/>
+    <sheetView tabSelected="1" topLeftCell="A499" workbookViewId="0">
+      <selection activeCell="F516" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
@@ -6026,7 +6051,7 @@
     <col min="13" max="13" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -6067,7 +6092,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>719</v>
       </c>
@@ -6103,7 +6128,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>717</v>
       </c>
@@ -6139,7 +6164,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>413</v>
       </c>
@@ -6175,7 +6200,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1088</v>
       </c>
@@ -6210,7 +6235,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>1241</v>
       </c>
@@ -6245,7 +6270,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>739</v>
       </c>
@@ -6281,7 +6306,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>710</v>
       </c>
@@ -6317,7 +6342,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>704</v>
       </c>
@@ -6353,7 +6378,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>731</v>
       </c>
@@ -6389,7 +6414,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>741</v>
       </c>
@@ -6425,7 +6450,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>712</v>
       </c>
@@ -6461,7 +6486,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>715</v>
       </c>
@@ -6497,7 +6522,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>726</v>
       </c>
@@ -6533,7 +6558,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>729</v>
       </c>
@@ -6569,7 +6594,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>721</v>
       </c>
@@ -6605,7 +6630,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>724</v>
       </c>
@@ -6641,7 +6666,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>736</v>
       </c>
@@ -6677,7 +6702,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>707</v>
       </c>
@@ -6713,7 +6738,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>734</v>
       </c>
@@ -6749,7 +6774,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>859</v>
       </c>
@@ -6784,7 +6809,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>370</v>
       </c>
@@ -6818,7 +6843,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>318</v>
       </c>
@@ -6852,7 +6877,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>863</v>
       </c>
@@ -6887,7 +6912,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>861</v>
       </c>
@@ -6922,7 +6947,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>857</v>
       </c>
@@ -6957,7 +6982,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>978</v>
       </c>
@@ -6992,7 +7017,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>669</v>
       </c>
@@ -7028,7 +7053,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>675</v>
       </c>
@@ -7064,7 +7089,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>690</v>
       </c>
@@ -7100,7 +7125,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>679</v>
       </c>
@@ -7136,7 +7161,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>683</v>
       </c>
@@ -7172,7 +7197,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>686</v>
       </c>
@@ -7208,7 +7233,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>865</v>
       </c>
@@ -7243,7 +7268,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>954</v>
       </c>
@@ -7278,7 +7303,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>956</v>
       </c>
@@ -7313,7 +7338,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>958</v>
       </c>
@@ -7348,7 +7373,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>1039</v>
       </c>
@@ -7379,7 +7404,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>1180</v>
       </c>
@@ -7416,7 +7441,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>263</v>
       </c>
@@ -7454,7 +7479,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>1057</v>
       </c>
@@ -7495,7 +7520,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>1167</v>
       </c>
@@ -7536,7 +7561,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>408</v>
       </c>
@@ -7574,7 +7599,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>693</v>
       </c>
@@ -7612,7 +7637,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>411</v>
       </c>
@@ -7650,7 +7675,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>1069</v>
       </c>
@@ -7691,7 +7716,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>1165</v>
       </c>
@@ -7732,7 +7757,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>1185</v>
       </c>
@@ -7769,7 +7794,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>919</v>
       </c>
@@ -7806,7 +7831,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>923</v>
       </c>
@@ -7843,7 +7868,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
@@ -7882,7 +7907,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>84</v>
       </c>
@@ -7920,7 +7945,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>1060</v>
       </c>
@@ -7959,7 +7984,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>1166</v>
       </c>
@@ -7998,7 +8023,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>340</v>
       </c>
@@ -8034,7 +8059,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>46</v>
       </c>
@@ -8073,7 +8098,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>982</v>
       </c>
@@ -8110,7 +8135,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>695</v>
       </c>
@@ -8148,7 +8173,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>700</v>
       </c>
@@ -8186,7 +8211,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>698</v>
       </c>
@@ -8224,7 +8249,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>90</v>
       </c>
@@ -8262,7 +8287,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>308</v>
       </c>
@@ -8298,7 +8323,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>1050</v>
       </c>
@@ -8339,7 +8364,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>1168</v>
       </c>
@@ -8380,7 +8405,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>311</v>
       </c>
@@ -8416,7 +8441,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>313</v>
       </c>
@@ -8452,7 +8477,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>383</v>
       </c>
@@ -8487,7 +8512,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>936</v>
       </c>
@@ -8524,7 +8549,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>702</v>
       </c>
@@ -8562,7 +8587,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>969</v>
       </c>
@@ -8599,7 +8624,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>795</v>
       </c>
@@ -8637,7 +8662,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>73</v>
       </c>
@@ -8674,7 +8699,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>75</v>
       </c>
@@ -8711,7 +8736,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>792</v>
       </c>
@@ -8749,7 +8774,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>1074</v>
       </c>
@@ -8786,7 +8811,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>790</v>
       </c>
@@ -8824,7 +8849,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>102</v>
       </c>
@@ -8859,7 +8884,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>274</v>
       </c>
@@ -8897,7 +8922,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>276</v>
       </c>
@@ -8935,7 +8960,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>278</v>
       </c>
@@ -8973,7 +8998,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>280</v>
       </c>
@@ -9011,7 +9036,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>282</v>
       </c>
@@ -9049,7 +9074,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>315</v>
       </c>
@@ -9087,7 +9112,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>322</v>
       </c>
@@ -9125,7 +9150,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>284</v>
       </c>
@@ -9163,7 +9188,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>286</v>
       </c>
@@ -9201,7 +9226,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>92</v>
       </c>
@@ -9236,7 +9261,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>68</v>
       </c>
@@ -9273,7 +9298,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>71</v>
       </c>
@@ -9308,7 +9333,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>97</v>
       </c>
@@ -9343,7 +9368,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>305</v>
       </c>
@@ -9379,7 +9404,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>376</v>
       </c>
@@ -9415,7 +9440,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>336</v>
       </c>
@@ -9451,7 +9476,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>368</v>
       </c>
@@ -9487,7 +9512,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>374</v>
       </c>
@@ -9522,7 +9547,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>77</v>
       </c>
@@ -9559,7 +9584,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>338</v>
       </c>
@@ -9592,7 +9617,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>107</v>
       </c>
@@ -9628,7 +9653,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>1091</v>
       </c>
@@ -9663,7 +9688,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>1072</v>
       </c>
@@ -9700,7 +9725,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>788</v>
       </c>
@@ -9738,7 +9763,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>271</v>
       </c>
@@ -9776,7 +9801,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>288</v>
       </c>
@@ -9814,7 +9839,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>79</v>
       </c>
@@ -9851,7 +9876,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>60</v>
       </c>
@@ -9888,7 +9913,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>63</v>
       </c>
@@ -9927,7 +9952,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>1093</v>
       </c>
@@ -9964,7 +9989,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>81</v>
       </c>
@@ -9999,7 +10024,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>366</v>
       </c>
@@ -10034,7 +10059,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>765</v>
       </c>
@@ -10072,7 +10097,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>781</v>
       </c>
@@ -10110,7 +10135,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>774</v>
       </c>
@@ -10148,7 +10173,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>770</v>
       </c>
@@ -10186,7 +10211,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>772</v>
       </c>
@@ -10224,7 +10249,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>754</v>
       </c>
@@ -10262,7 +10287,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>52</v>
       </c>
@@ -10301,7 +10326,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>761</v>
       </c>
@@ -10339,7 +10364,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>749</v>
       </c>
@@ -10377,7 +10402,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>768</v>
       </c>
@@ -10415,7 +10440,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>759</v>
       </c>
@@ -10453,7 +10478,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>763</v>
       </c>
@@ -10491,7 +10516,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>752</v>
       </c>
@@ -10529,7 +10554,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>757</v>
       </c>
@@ -10567,7 +10592,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>1076</v>
       </c>
@@ -10604,7 +10629,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>250</v>
       </c>
@@ -10642,7 +10667,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>38</v>
       </c>
@@ -10677,7 +10702,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>41</v>
       </c>
@@ -10712,7 +10737,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>868</v>
       </c>
@@ -10749,7 +10774,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>100</v>
       </c>
@@ -10781,7 +10806,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>1078</v>
       </c>
@@ -10818,7 +10843,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>1079</v>
       </c>
@@ -10855,7 +10880,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>779</v>
       </c>
@@ -10893,7 +10918,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>776</v>
       </c>
@@ -10931,7 +10956,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>786</v>
       </c>
@@ -10969,7 +10994,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>784</v>
       </c>
@@ -11007,7 +11032,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>781</v>
       </c>
@@ -11045,7 +11070,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>359</v>
       </c>
@@ -11081,7 +11106,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>362</v>
       </c>
@@ -11117,7 +11142,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>364</v>
       </c>
@@ -11153,7 +11178,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>1220</v>
       </c>
@@ -11194,7 +11219,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>242</v>
       </c>
@@ -11235,7 +11260,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>391</v>
       </c>
@@ -11273,7 +11298,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>1134</v>
       </c>
@@ -11312,7 +11337,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>209</v>
       </c>
@@ -11351,7 +11376,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>419</v>
       </c>
@@ -11389,7 +11414,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>797</v>
       </c>
@@ -11427,7 +11452,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>21</v>
       </c>
@@ -11463,7 +11488,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>25</v>
       </c>
@@ -11499,7 +11524,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>812</v>
       </c>
@@ -11534,7 +11559,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>900</v>
       </c>
@@ -11571,7 +11596,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>1035</v>
       </c>
@@ -11610,7 +11635,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>227</v>
       </c>
@@ -11651,7 +11676,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>139</v>
       </c>
@@ -11677,7 +11702,7 @@
         <v>1327</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="J153" s="2" t="s">
         <v>1105</v>
@@ -11692,7 +11717,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>1041</v>
       </c>
@@ -11731,7 +11756,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>1228</v>
       </c>
@@ -11769,7 +11794,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>990</v>
       </c>
@@ -11806,7 +11831,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>164</v>
       </c>
@@ -11847,7 +11872,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>911</v>
       </c>
@@ -11886,7 +11911,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>913</v>
       </c>
@@ -11925,7 +11950,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>906</v>
       </c>
@@ -11964,7 +11989,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>1212</v>
       </c>
@@ -12005,7 +12030,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>1043</v>
       </c>
@@ -12044,7 +12069,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>1042</v>
       </c>
@@ -12083,7 +12108,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>1200</v>
       </c>
@@ -12124,7 +12149,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>992</v>
       </c>
@@ -12161,7 +12186,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>1017</v>
       </c>
@@ -12198,7 +12223,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>909</v>
       </c>
@@ -12237,7 +12262,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>915</v>
       </c>
@@ -12276,7 +12301,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>915</v>
       </c>
@@ -12315,7 +12340,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>883</v>
       </c>
@@ -12354,7 +12379,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>886</v>
       </c>
@@ -12393,7 +12418,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>917</v>
       </c>
@@ -12432,7 +12457,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>994</v>
       </c>
@@ -12469,7 +12494,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>1027</v>
       </c>
@@ -12506,7 +12531,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>1031</v>
       </c>
@@ -12543,7 +12568,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>174</v>
       </c>
@@ -12584,7 +12609,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>185</v>
       </c>
@@ -12625,7 +12650,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>123</v>
       </c>
@@ -12666,7 +12691,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>224</v>
       </c>
@@ -12705,7 +12730,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>151</v>
       </c>
@@ -12746,7 +12771,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>215</v>
       </c>
@@ -12787,7 +12812,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>144</v>
       </c>
@@ -12828,7 +12853,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>157</v>
       </c>
@@ -12869,7 +12894,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>189</v>
       </c>
@@ -12910,7 +12935,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>246</v>
       </c>
@@ -12951,7 +12976,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>142</v>
       </c>
@@ -12992,7 +13017,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>199</v>
       </c>
@@ -13033,7 +13058,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>172</v>
       </c>
@@ -13074,7 +13099,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>222</v>
       </c>
@@ -13115,7 +13140,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>181</v>
       </c>
@@ -13156,7 +13181,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>149</v>
       </c>
@@ -13197,7 +13222,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>111</v>
       </c>
@@ -13238,7 +13263,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>137</v>
       </c>
@@ -13279,7 +13304,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>187</v>
       </c>
@@ -13320,7 +13345,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>218</v>
       </c>
@@ -13361,7 +13386,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>238</v>
       </c>
@@ -13402,7 +13427,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>225</v>
       </c>
@@ -13443,7 +13468,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>120</v>
       </c>
@@ -13481,7 +13506,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>220</v>
       </c>
@@ -13522,7 +13547,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>183</v>
       </c>
@@ -13563,7 +13588,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>195</v>
       </c>
@@ -13604,7 +13629,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>1113</v>
       </c>
@@ -13645,7 +13670,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>1156</v>
       </c>
@@ -13686,7 +13711,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>1136</v>
       </c>
@@ -13727,7 +13752,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>1103</v>
       </c>
@@ -13768,7 +13793,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>1139</v>
       </c>
@@ -13809,7 +13834,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>1115</v>
       </c>
@@ -13850,7 +13875,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>1106</v>
       </c>
@@ -13891,7 +13916,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>1129</v>
       </c>
@@ -13932,7 +13957,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>1158</v>
       </c>
@@ -13973,7 +13998,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>206</v>
       </c>
@@ -14014,7 +14039,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
         <v>1144</v>
       </c>
@@ -14053,7 +14078,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>1125</v>
       </c>
@@ -14094,7 +14119,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>1132</v>
       </c>
@@ -14135,7 +14160,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>1142</v>
       </c>
@@ -14176,7 +14201,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>1127</v>
       </c>
@@ -14217,7 +14242,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>1111</v>
       </c>
@@ -14258,7 +14283,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
         <v>1130</v>
       </c>
@@ -14299,7 +14324,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>1046</v>
       </c>
@@ -14340,7 +14365,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>233</v>
       </c>
@@ -14381,7 +14406,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>230</v>
       </c>
@@ -14422,7 +14447,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
         <v>998</v>
       </c>
@@ -14461,7 +14486,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
         <v>245</v>
       </c>
@@ -14502,7 +14527,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
         <v>191</v>
       </c>
@@ -14543,7 +14568,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>136</v>
       </c>
@@ -14584,7 +14609,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
         <v>179</v>
       </c>
@@ -14625,7 +14650,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
         <v>1037</v>
       </c>
@@ -14664,7 +14689,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
         <v>879</v>
       </c>
@@ -14703,7 +14728,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>204</v>
       </c>
@@ -14744,7 +14769,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
         <v>1159</v>
       </c>
@@ -14785,7 +14810,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>1117</v>
       </c>
@@ -14826,7 +14851,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
         <v>1122</v>
       </c>
@@ -14867,7 +14892,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="233" spans="1:13">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
         <v>996</v>
       </c>
@@ -14904,7 +14929,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
         <v>1099</v>
       </c>
@@ -14945,7 +14970,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
         <v>1101</v>
       </c>
@@ -14986,7 +15011,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="236" spans="1:13">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
         <v>1096</v>
       </c>
@@ -15027,7 +15052,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>827</v>
       </c>
@@ -15062,7 +15087,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="238" spans="1:13" ht="17" customHeight="1">
+    <row r="238" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
         <v>830</v>
       </c>
@@ -15097,7 +15122,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="239" spans="1:13">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>832</v>
       </c>
@@ -15132,7 +15157,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
         <v>834</v>
       </c>
@@ -15167,7 +15192,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>821</v>
       </c>
@@ -15197,7 +15222,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
         <v>824</v>
       </c>
@@ -15227,7 +15252,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>825</v>
       </c>
@@ -15260,7 +15285,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
         <v>162</v>
       </c>
@@ -15301,7 +15326,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
         <v>133</v>
       </c>
@@ -15342,7 +15367,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
         <v>1019</v>
       </c>
@@ -15379,7 +15404,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
         <v>1222</v>
       </c>
@@ -15420,7 +15445,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
         <v>1012</v>
       </c>
@@ -15459,7 +15484,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
         <v>1206</v>
       </c>
@@ -15500,7 +15525,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
         <v>201</v>
       </c>
@@ -15541,7 +15566,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
         <v>1010</v>
       </c>
@@ -15578,7 +15603,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
         <v>817</v>
       </c>
@@ -15608,7 +15633,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
         <v>820</v>
       </c>
@@ -15638,7 +15663,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
         <v>155</v>
       </c>
@@ -15679,7 +15704,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
         <v>152</v>
       </c>
@@ -15720,7 +15745,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
         <v>1218</v>
       </c>
@@ -15761,7 +15786,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="257" spans="1:13">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>117</v>
       </c>
@@ -15802,7 +15827,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
         <v>1216</v>
       </c>
@@ -15843,7 +15868,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
         <v>1005</v>
       </c>
@@ -15880,7 +15905,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="260" spans="1:13">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
         <v>1210</v>
       </c>
@@ -15921,7 +15946,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
         <v>1008</v>
       </c>
@@ -15958,7 +15983,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="262" spans="1:13">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
         <v>1029</v>
       </c>
@@ -15995,7 +16020,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="263" spans="1:13">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
         <v>1254</v>
       </c>
@@ -16032,7 +16057,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="264" spans="1:13">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
         <v>128</v>
       </c>
@@ -16073,7 +16098,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="265" spans="1:13">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
         <v>146</v>
       </c>
@@ -16114,7 +16139,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="266" spans="1:13">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
         <v>167</v>
       </c>
@@ -16155,7 +16180,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="267" spans="1:13">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
         <v>160</v>
       </c>
@@ -16196,7 +16221,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="268" spans="1:13">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
         <v>216</v>
       </c>
@@ -16237,7 +16262,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="269" spans="1:13">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
         <v>892</v>
       </c>
@@ -16276,7 +16301,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="270" spans="1:13">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
         <v>888</v>
       </c>
@@ -16315,7 +16340,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="271" spans="1:13">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
         <v>898</v>
       </c>
@@ -16354,7 +16379,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="272" spans="1:13">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
         <v>895</v>
       </c>
@@ -16393,7 +16418,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="273" spans="1:13">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
         <v>1163</v>
       </c>
@@ -16434,7 +16459,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A274" s="2" t="s">
         <v>1234</v>
       </c>
@@ -16475,7 +16500,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="275" spans="1:13">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
         <v>1161</v>
       </c>
@@ -16516,7 +16541,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A276" s="2" t="s">
         <v>1233</v>
       </c>
@@ -16557,7 +16582,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
         <v>1202</v>
       </c>
@@ -16595,7 +16620,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="278" spans="1:13">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A278" s="2" t="s">
         <v>1015</v>
       </c>
@@ -16629,7 +16654,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="279" spans="1:13">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A279" s="2" t="s">
         <v>1003</v>
       </c>
@@ -16666,7 +16691,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="280" spans="1:13">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A280" s="2" t="s">
         <v>1021</v>
       </c>
@@ -16703,7 +16728,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="281" spans="1:13">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A281" s="2" t="s">
         <v>1023</v>
       </c>
@@ -16740,7 +16765,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="282" spans="1:13">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
         <v>1231</v>
       </c>
@@ -16781,7 +16806,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
         <v>1204</v>
       </c>
@@ -16819,7 +16844,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="284" spans="1:13">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A284" s="2" t="s">
         <v>873</v>
       </c>
@@ -16855,7 +16880,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="285" spans="1:13">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
         <v>877</v>
       </c>
@@ -16891,7 +16916,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="286" spans="1:13">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A286" s="2" t="s">
         <v>1001</v>
       </c>
@@ -16928,7 +16953,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="287" spans="1:13">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
         <v>1025</v>
       </c>
@@ -16965,7 +16990,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="288" spans="1:13">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A288" s="2" t="s">
         <v>1033</v>
       </c>
@@ -17002,7 +17027,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="289" spans="1:13">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A289" s="2" t="s">
         <v>208</v>
       </c>
@@ -17043,7 +17068,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="290" spans="1:13">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>232</v>
       </c>
@@ -17084,7 +17109,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="291" spans="1:13">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A291" s="2" t="s">
         <v>43</v>
       </c>
@@ -17123,7 +17148,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="292" spans="1:13">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A292" s="2" t="s">
         <v>169</v>
       </c>
@@ -17164,7 +17189,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="293" spans="1:13">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A293" s="2" t="s">
         <v>1214</v>
       </c>
@@ -17205,7 +17230,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="294" spans="1:13">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A294" s="2" t="s">
         <v>1226</v>
       </c>
@@ -17246,7 +17271,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="295" spans="1:13">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A295" s="2" t="s">
         <v>1208</v>
       </c>
@@ -17287,7 +17312,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="296" spans="1:13">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>799</v>
       </c>
@@ -17325,7 +17350,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="297" spans="1:13">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A297" s="2" t="s">
         <v>1083</v>
       </c>
@@ -17362,7 +17387,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="298" spans="1:13">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A298" s="2" t="s">
         <v>902</v>
       </c>
@@ -17396,7 +17421,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="299" spans="1:13">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>614</v>
       </c>
@@ -17434,7 +17459,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="300" spans="1:13">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>610</v>
       </c>
@@ -17472,7 +17497,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="301" spans="1:13">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>618</v>
       </c>
@@ -17510,7 +17535,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="302" spans="1:13">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>629</v>
       </c>
@@ -17548,7 +17573,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="303" spans="1:13">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
         <v>627</v>
       </c>
@@ -17586,7 +17611,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="304" spans="1:13">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A304" s="2" t="s">
         <v>1245</v>
       </c>
@@ -17623,7 +17648,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="305" spans="1:13">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>612</v>
       </c>
@@ -17661,7 +17686,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="306" spans="1:13">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>616</v>
       </c>
@@ -17699,7 +17724,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="307" spans="1:13">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>624</v>
       </c>
@@ -17737,7 +17762,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="308" spans="1:13">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>621</v>
       </c>
@@ -17775,7 +17800,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="309" spans="1:13">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
         <v>631</v>
       </c>
@@ -17813,7 +17838,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="310" spans="1:13">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A310" s="2" t="s">
         <v>848</v>
       </c>
@@ -17850,7 +17875,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="311" spans="1:13">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A311" s="2" t="s">
         <v>851</v>
       </c>
@@ -17887,7 +17912,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="312" spans="1:13">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>353</v>
       </c>
@@ -17923,7 +17948,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="313" spans="1:13">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>386</v>
       </c>
@@ -17959,7 +17984,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="314" spans="1:13">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A314" s="2" t="s">
         <v>845</v>
       </c>
@@ -17996,7 +18021,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="315" spans="1:13">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A315" s="2" t="s">
         <v>975</v>
       </c>
@@ -18033,7 +18058,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="316" spans="1:13">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A316" s="2" t="s">
         <v>984</v>
       </c>
@@ -18068,7 +18093,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="317" spans="1:13">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>644</v>
       </c>
@@ -18106,7 +18131,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="318" spans="1:13">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>292</v>
       </c>
@@ -18141,7 +18166,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="319" spans="1:13">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
         <v>297</v>
       </c>
@@ -18176,7 +18201,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="320" spans="1:13">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>299</v>
       </c>
@@ -18211,7 +18236,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="321" spans="1:13">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
         <v>303</v>
       </c>
@@ -18246,7 +18271,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="322" spans="1:13">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>634</v>
       </c>
@@ -18284,7 +18309,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="323" spans="1:13">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A323" s="2" t="s">
         <v>1243</v>
       </c>
@@ -18321,7 +18346,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="324" spans="1:13">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>401</v>
       </c>
@@ -18359,7 +18384,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="325" spans="1:13">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>647</v>
       </c>
@@ -18397,7 +18422,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="326" spans="1:13">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>637</v>
       </c>
@@ -18435,7 +18460,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="327" spans="1:13">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A327" s="2" t="s">
         <v>1248</v>
       </c>
@@ -18472,7 +18497,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="328" spans="1:13">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>639</v>
       </c>
@@ -18510,7 +18535,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="329" spans="1:13">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
         <v>642</v>
       </c>
@@ -18548,7 +18573,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="330" spans="1:13">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>356</v>
       </c>
@@ -18584,7 +18609,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="331" spans="1:13">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A331" s="2" t="s">
         <v>952</v>
       </c>
@@ -18621,7 +18646,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="332" spans="1:13">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A332" s="2" t="s">
         <v>986</v>
       </c>
@@ -18656,7 +18681,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="333" spans="1:13">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>649</v>
       </c>
@@ -18694,7 +18719,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="334" spans="1:13">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>654</v>
       </c>
@@ -18732,7 +18757,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="335" spans="1:13">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
         <v>652</v>
       </c>
@@ -18770,7 +18795,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="336" spans="1:13">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A336" s="2" t="s">
         <v>855</v>
       </c>
@@ -18807,7 +18832,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="337" spans="1:13">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
         <v>396</v>
       </c>
@@ -18845,7 +18870,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="338" spans="1:13">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>345</v>
       </c>
@@ -18878,7 +18903,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="339" spans="1:13">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
         <v>33</v>
       </c>
@@ -18914,7 +18939,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="340" spans="1:13">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A340" s="2" t="s">
         <v>1177</v>
       </c>
@@ -18951,7 +18976,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="341" spans="1:13">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A341" s="2" t="s">
         <v>940</v>
       </c>
@@ -18988,7 +19013,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="342" spans="1:13">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A342" s="2" t="s">
         <v>938</v>
       </c>
@@ -19025,7 +19050,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="343" spans="1:13">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
         <v>658</v>
       </c>
@@ -19063,7 +19088,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="344" spans="1:13">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>235</v>
       </c>
@@ -19098,7 +19123,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="345" spans="1:13">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A345" s="2" t="s">
         <v>193</v>
       </c>
@@ -19139,7 +19164,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="346" spans="1:13">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A346" s="2" t="s">
         <v>1172</v>
       </c>
@@ -19178,7 +19203,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="347" spans="1:13">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>425</v>
       </c>
@@ -19216,7 +19241,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="348" spans="1:13">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>421</v>
       </c>
@@ -19254,7 +19279,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="349" spans="1:13">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
         <v>423</v>
       </c>
@@ -19292,7 +19317,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="350" spans="1:13">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>399</v>
       </c>
@@ -19330,7 +19355,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="351" spans="1:13">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A351" s="2" t="s">
         <v>1183</v>
       </c>
@@ -19369,7 +19394,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="352" spans="1:13">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>94</v>
       </c>
@@ -19402,7 +19427,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="353" spans="1:13">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A353" s="2" t="s">
         <v>853</v>
       </c>
@@ -19439,7 +19464,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="354" spans="1:13">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A354" s="2" t="s">
         <v>944</v>
       </c>
@@ -19478,7 +19503,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="355" spans="1:13">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A355" s="2" t="s">
         <v>988</v>
       </c>
@@ -19517,7 +19542,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="356" spans="1:13">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>665</v>
       </c>
@@ -19555,7 +19580,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="357" spans="1:13">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
         <v>663</v>
       </c>
@@ -19593,7 +19618,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="358" spans="1:13">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>661</v>
       </c>
@@ -19631,7 +19656,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="359" spans="1:13">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>333</v>
       </c>
@@ -19669,7 +19694,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="360" spans="1:13">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A360" s="2" t="s">
         <v>964</v>
       </c>
@@ -19706,7 +19731,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="361" spans="1:13">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
         <v>14</v>
       </c>
@@ -19741,7 +19766,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="362" spans="1:13">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>667</v>
       </c>
@@ -19779,7 +19804,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="363" spans="1:13">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A363" s="2" t="s">
         <v>7</v>
       </c>
@@ -19818,7 +19843,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="364" spans="1:13">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>19</v>
       </c>
@@ -19853,7 +19878,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="365" spans="1:13">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A365" s="2" t="s">
         <v>966</v>
       </c>
@@ -19890,7 +19915,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="366" spans="1:13">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>259</v>
       </c>
@@ -19928,7 +19953,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="367" spans="1:13">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
         <v>325</v>
       </c>
@@ -19964,7 +19989,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="368" spans="1:13">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>327</v>
       </c>
@@ -20000,7 +20025,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="369" spans="1:13">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
         <v>329</v>
       </c>
@@ -20036,7 +20061,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="370" spans="1:13">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>331</v>
       </c>
@@ -20072,7 +20097,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="371" spans="1:13">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
         <v>530</v>
       </c>
@@ -20110,7 +20135,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="372" spans="1:13">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A372" s="2" t="s">
         <v>962</v>
       </c>
@@ -20147,7 +20172,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="373" spans="1:13">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A373" s="2" t="s">
         <v>931</v>
       </c>
@@ -20184,7 +20209,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="374" spans="1:13">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>380</v>
       </c>
@@ -20222,7 +20247,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="375" spans="1:13">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
         <v>261</v>
       </c>
@@ -20260,7 +20285,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="376" spans="1:13">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
         <v>656</v>
       </c>
@@ -20298,7 +20323,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="377" spans="1:13">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
         <v>350</v>
       </c>
@@ -20334,7 +20359,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="378" spans="1:13">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>267</v>
       </c>
@@ -20372,7 +20397,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="379" spans="1:13">
+    <row r="379" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
         <v>535</v>
       </c>
@@ -20410,7 +20435,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="380" spans="1:13">
+    <row r="380" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A380" s="2" t="s">
         <v>837</v>
       </c>
@@ -20447,7 +20472,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="381" spans="1:13">
+    <row r="381" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A381" s="1" t="s">
         <v>427</v>
       </c>
@@ -20485,7 +20510,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="382" spans="1:13">
+    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
         <v>451</v>
       </c>
@@ -20523,7 +20548,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="383" spans="1:13">
+    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
         <v>447</v>
       </c>
@@ -20561,7 +20586,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="384" spans="1:13">
+    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
         <v>449</v>
       </c>
@@ -20599,7 +20624,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="385" spans="1:13">
+    <row r="385" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
         <v>441</v>
       </c>
@@ -20637,7 +20662,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="386" spans="1:13">
+    <row r="386" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
         <v>445</v>
       </c>
@@ -20675,7 +20700,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="387" spans="1:13">
+    <row r="387" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
         <v>439</v>
       </c>
@@ -20713,7 +20738,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="388" spans="1:13">
+    <row r="388" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
         <v>430</v>
       </c>
@@ -20751,7 +20776,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="389" spans="1:13">
+    <row r="389" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A389" s="1" t="s">
         <v>443</v>
       </c>
@@ -20789,7 +20814,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="390" spans="1:13">
+    <row r="390" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
         <v>433</v>
       </c>
@@ -20827,7 +20852,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="391" spans="1:13">
+    <row r="391" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A391" s="1" t="s">
         <v>435</v>
       </c>
@@ -20865,7 +20890,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="392" spans="1:13">
+    <row r="392" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A392" s="1" t="s">
         <v>437</v>
       </c>
@@ -20903,7 +20928,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="393" spans="1:13">
+    <row r="393" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A393" s="2" t="s">
         <v>843</v>
       </c>
@@ -20940,7 +20965,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="394" spans="1:13">
+    <row r="394" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
         <v>404</v>
       </c>
@@ -20978,7 +21003,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="395" spans="1:13">
+    <row r="395" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
         <v>537</v>
       </c>
@@ -21016,7 +21041,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="396" spans="1:13">
+    <row r="396" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A396" s="2" t="s">
         <v>840</v>
       </c>
@@ -21053,7 +21078,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="397" spans="1:13">
+    <row r="397" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A397" s="2" t="s">
         <v>1250</v>
       </c>
@@ -21088,7 +21113,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="398" spans="1:13">
+    <row r="398" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
         <v>499</v>
       </c>
@@ -21126,7 +21151,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="399" spans="1:13">
+    <row r="399" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A399" s="1" t="s">
         <v>488</v>
       </c>
@@ -21164,7 +21189,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="400" spans="1:13">
+    <row r="400" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A400" s="1" t="s">
         <v>495</v>
       </c>
@@ -21202,7 +21227,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="401" spans="1:13">
+    <row r="401" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A401" s="1" t="s">
         <v>479</v>
       </c>
@@ -21240,7 +21265,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="402" spans="1:13">
+    <row r="402" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
         <v>482</v>
       </c>
@@ -21278,7 +21303,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="403" spans="1:13">
+    <row r="403" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
         <v>484</v>
       </c>
@@ -21316,7 +21341,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="404" spans="1:13">
+    <row r="404" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
         <v>486</v>
       </c>
@@ -21354,7 +21379,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="405" spans="1:13">
+    <row r="405" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
         <v>497</v>
       </c>
@@ -21392,7 +21417,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="406" spans="1:13">
+    <row r="406" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
         <v>491</v>
       </c>
@@ -21430,7 +21455,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="407" spans="1:13">
+    <row r="407" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
         <v>493</v>
       </c>
@@ -21468,7 +21493,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="408" spans="1:13">
+    <row r="408" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
         <v>572</v>
       </c>
@@ -21506,7 +21531,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="409" spans="1:13">
+    <row r="409" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
         <v>575</v>
       </c>
@@ -21541,7 +21566,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="410" spans="1:13">
+    <row r="410" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
         <v>602</v>
       </c>
@@ -21579,7 +21604,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="411" spans="1:13">
+    <row r="411" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
         <v>596</v>
       </c>
@@ -21617,7 +21642,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="412" spans="1:13">
+    <row r="412" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
         <v>552</v>
       </c>
@@ -21655,7 +21680,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="413" spans="1:13">
+    <row r="413" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A413" s="1" t="s">
         <v>566</v>
       </c>
@@ -21693,7 +21718,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="414" spans="1:13">
+    <row r="414" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A414" s="2" t="s">
         <v>1239</v>
       </c>
@@ -21730,7 +21755,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="415" spans="1:13">
+    <row r="415" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A415" s="2" t="s">
         <v>1237</v>
       </c>
@@ -21767,7 +21792,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="416" spans="1:13">
+    <row r="416" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A416" s="1" t="s">
         <v>563</v>
       </c>
@@ -21805,7 +21830,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="417" spans="1:13">
+    <row r="417" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A417" s="1" t="s">
         <v>556</v>
       </c>
@@ -21843,7 +21868,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="418" spans="1:13">
+    <row r="418" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
         <v>561</v>
       </c>
@@ -21881,7 +21906,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="419" spans="1:13">
+    <row r="419" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A419" s="2" t="s">
         <v>1235</v>
       </c>
@@ -21918,7 +21943,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="420" spans="1:13">
+    <row r="420" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A420" s="1" t="s">
         <v>604</v>
       </c>
@@ -21956,7 +21981,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="421" spans="1:13">
+    <row r="421" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A421" s="1" t="s">
         <v>600</v>
       </c>
@@ -21994,7 +22019,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="422" spans="1:13">
+    <row r="422" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A422" s="1" t="s">
         <v>583</v>
       </c>
@@ -22032,7 +22057,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="423" spans="1:13">
+    <row r="423" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A423" s="1" t="s">
         <v>589</v>
       </c>
@@ -22070,7 +22095,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="424" spans="1:13">
+    <row r="424" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A424" s="1" t="s">
         <v>593</v>
       </c>
@@ -22108,7 +22133,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="425" spans="1:13">
+    <row r="425" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A425" s="1" t="s">
         <v>578</v>
       </c>
@@ -22146,7 +22171,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="426" spans="1:13">
+    <row r="426" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A426" s="1" t="s">
         <v>587</v>
       </c>
@@ -22184,7 +22209,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="427" spans="1:13">
+    <row r="427" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
         <v>585</v>
       </c>
@@ -22222,7 +22247,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="428" spans="1:13">
+    <row r="428" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
         <v>580</v>
       </c>
@@ -22260,7 +22285,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="429" spans="1:13">
+    <row r="429" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A429" s="1" t="s">
         <v>576</v>
       </c>
@@ -22298,7 +22323,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="430" spans="1:13">
+    <row r="430" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A430" s="1" t="s">
         <v>598</v>
       </c>
@@ -22336,7 +22361,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="431" spans="1:13">
+    <row r="431" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A431" s="1" t="s">
         <v>591</v>
       </c>
@@ -22374,7 +22399,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="432" spans="1:13">
+    <row r="432" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A432" s="1" t="s">
         <v>568</v>
       </c>
@@ -22412,7 +22437,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="433" spans="1:13">
+    <row r="433" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A433" s="1" t="s">
         <v>570</v>
       </c>
@@ -22450,7 +22475,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="434" spans="1:13">
+    <row r="434" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A434" s="1" t="s">
         <v>572</v>
       </c>
@@ -22488,7 +22513,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="435" spans="1:13">
+    <row r="435" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A435" s="2" t="s">
         <v>934</v>
       </c>
@@ -22523,7 +22548,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="436" spans="1:13">
+    <row r="436" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A436" s="1" t="s">
         <v>606</v>
       </c>
@@ -22561,7 +22586,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="437" spans="1:13">
+    <row r="437" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A437" s="1" t="s">
         <v>608</v>
       </c>
@@ -22599,7 +22624,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="438" spans="1:13">
+    <row r="438" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
         <v>544</v>
       </c>
@@ -22637,7 +22662,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="439" spans="1:13">
+    <row r="439" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A439" s="1" t="s">
         <v>548</v>
       </c>
@@ -22675,7 +22700,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="440" spans="1:13">
+    <row r="440" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A440" s="1" t="s">
         <v>539</v>
       </c>
@@ -22713,7 +22738,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="441" spans="1:13">
+    <row r="441" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A441" s="1" t="s">
         <v>550</v>
       </c>
@@ -22751,7 +22776,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="442" spans="1:13">
+    <row r="442" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A442" s="1" t="s">
         <v>546</v>
       </c>
@@ -22789,7 +22814,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="443" spans="1:13">
+    <row r="443" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A443" s="1" t="s">
         <v>542</v>
       </c>
@@ -22827,7 +22852,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="444" spans="1:13">
+    <row r="444" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A444" s="2" t="s">
         <v>980</v>
       </c>
@@ -22864,7 +22889,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="445" spans="1:13">
+    <row r="445" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A445" s="1" t="s">
         <v>252</v>
       </c>
@@ -22902,7 +22927,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="446" spans="1:13">
+    <row r="446" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A446" s="1" t="s">
         <v>508</v>
       </c>
@@ -22940,7 +22965,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="447" spans="1:13">
+    <row r="447" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A447" s="1" t="s">
         <v>510</v>
       </c>
@@ -22978,7 +23003,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="448" spans="1:13">
+    <row r="448" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
         <v>522</v>
       </c>
@@ -23016,7 +23041,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="449" spans="1:13">
+    <row r="449" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
         <v>524</v>
       </c>
@@ -23054,7 +23079,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="450" spans="1:13">
+    <row r="450" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
         <v>526</v>
       </c>
@@ -23092,7 +23117,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="451" spans="1:13">
+    <row r="451" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
         <v>503</v>
       </c>
@@ -23130,7 +23155,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="452" spans="1:13">
+    <row r="452" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>506</v>
       </c>
@@ -23168,7 +23193,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="453" spans="1:13">
+    <row r="453" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
         <v>528</v>
       </c>
@@ -23206,7 +23231,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="454" spans="1:13">
+    <row r="454" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A454" s="2" t="s">
         <v>1253</v>
       </c>
@@ -23243,7 +23268,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="455" spans="1:13">
+    <row r="455" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
         <v>512</v>
       </c>
@@ -23281,7 +23306,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="456" spans="1:13">
+    <row r="456" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
         <v>514</v>
       </c>
@@ -23319,7 +23344,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="457" spans="1:13">
+    <row r="457" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A457" s="1" t="s">
         <v>518</v>
       </c>
@@ -23357,7 +23382,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="458" spans="1:13">
+    <row r="458" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
         <v>516</v>
       </c>
@@ -23395,7 +23420,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="459" spans="1:13">
+    <row r="459" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A459" s="1" t="s">
         <v>520</v>
       </c>
@@ -23433,7 +23458,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="460" spans="1:13">
+    <row r="460" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A460" s="2" t="s">
         <v>1054</v>
       </c>
@@ -23474,7 +23499,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="461" spans="1:13">
+    <row r="461" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
         <v>342</v>
       </c>
@@ -23507,7 +23532,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="462" spans="1:13">
+    <row r="462" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A462" s="2" t="s">
         <v>1169</v>
       </c>
@@ -23546,7 +23571,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="463" spans="1:13">
+    <row r="463" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A463" s="2" t="s">
         <v>1198</v>
       </c>
@@ -23585,7 +23610,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="464" spans="1:13">
+    <row r="464" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A464" s="2" t="s">
         <v>192</v>
       </c>
@@ -23610,8 +23635,8 @@
       <c r="H464" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="I464" s="6" t="s">
-        <v>1150</v>
+      <c r="I464" s="19" t="s">
+        <v>1361</v>
       </c>
       <c r="J464" s="2" t="s">
         <v>12</v>
@@ -23626,7 +23651,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="465" spans="1:13">
+    <row r="465" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A465" s="2" t="s">
         <v>125</v>
       </c>
@@ -23667,7 +23692,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="466" spans="1:13">
+    <row r="466" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A466" s="2" t="s">
         <v>115</v>
       </c>
@@ -23708,7 +23733,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="467" spans="1:13">
+    <row r="467" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A467" s="2" t="s">
         <v>240</v>
       </c>
@@ -23733,8 +23758,8 @@
       <c r="H467" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="I467" s="6" t="s">
-        <v>1150</v>
+      <c r="I467" s="19" t="s">
+        <v>1362</v>
       </c>
       <c r="J467" s="2" t="s">
         <v>12</v>
@@ -23749,7 +23774,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="468" spans="1:13">
+    <row r="468" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A468" s="2" t="s">
         <v>248</v>
       </c>
@@ -23788,7 +23813,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="469" spans="1:13">
+    <row r="469" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A469" s="1" t="s">
         <v>806</v>
       </c>
@@ -23823,7 +23848,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="470" spans="1:13">
+    <row r="470" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
         <v>802</v>
       </c>
@@ -23858,7 +23883,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="471" spans="1:13">
+    <row r="471" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A471" s="1" t="s">
         <v>472</v>
       </c>
@@ -23896,7 +23921,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="472" spans="1:13">
+    <row r="472" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A472" s="2" t="s">
         <v>1252</v>
       </c>
@@ -23933,7 +23958,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="473" spans="1:13">
+    <row r="473" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A473" s="1" t="s">
         <v>459</v>
       </c>
@@ -23971,7 +23996,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="474" spans="1:13">
+    <row r="474" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A474" s="2" t="s">
         <v>1081</v>
       </c>
@@ -24008,7 +24033,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="475" spans="1:13">
+    <row r="475" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A475" s="1" t="s">
         <v>477</v>
       </c>
@@ -24046,7 +24071,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="476" spans="1:13">
+    <row r="476" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A476" s="1" t="s">
         <v>461</v>
       </c>
@@ -24084,7 +24109,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="477" spans="1:13">
+    <row r="477" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A477" s="1" t="s">
         <v>475</v>
       </c>
@@ -24122,7 +24147,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="478" spans="1:13">
+    <row r="478" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A478" s="1" t="s">
         <v>453</v>
       </c>
@@ -24160,7 +24185,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="479" spans="1:13">
+    <row r="479" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A479" s="1" t="s">
         <v>468</v>
       </c>
@@ -24198,7 +24223,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="480" spans="1:13">
+    <row r="480" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A480" s="1" t="s">
         <v>463</v>
       </c>
@@ -24236,7 +24261,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="481" spans="1:13">
+    <row r="481" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A481" s="1" t="s">
         <v>470</v>
       </c>
@@ -24274,7 +24299,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="482" spans="1:13">
+    <row r="482" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A482" s="1" t="s">
         <v>466</v>
       </c>
@@ -24312,7 +24337,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="483" spans="1:13">
+    <row r="483" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A483" s="1" t="s">
         <v>472</v>
       </c>
@@ -24350,7 +24375,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="484" spans="1:13">
+    <row r="484" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A484" s="1" t="s">
         <v>456</v>
       </c>
@@ -24388,7 +24413,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="485" spans="1:13">
+    <row r="485" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A485" s="2" t="s">
         <v>925</v>
       </c>
@@ -24425,7 +24450,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="486" spans="1:13">
+    <row r="486" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A486" s="2" t="s">
         <v>928</v>
       </c>
@@ -24462,7 +24487,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="487" spans="1:13">
+    <row r="487" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A487" s="1" t="s">
         <v>744</v>
       </c>
@@ -24498,7 +24523,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="488" spans="1:13">
+    <row r="488" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A488" s="1" t="s">
         <v>416</v>
       </c>
@@ -24534,7 +24559,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="489" spans="1:13">
+    <row r="489" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A489" s="1" t="s">
         <v>747</v>
       </c>
@@ -24570,7 +24595,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="490" spans="1:13">
+    <row r="490" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A490" s="1" t="s">
         <v>28</v>
       </c>
@@ -24604,7 +24629,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="491" spans="1:13">
+    <row r="491" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A491" s="2" t="s">
         <v>960</v>
       </c>
@@ -24639,7 +24664,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="492" spans="1:13">
+    <row r="492" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A492" s="2" t="s">
         <v>871</v>
       </c>
@@ -24674,7 +24699,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="493" spans="1:13">
+    <row r="493" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A493" s="1" t="s">
         <v>348</v>
       </c>
@@ -24708,7 +24733,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="494" spans="1:13">
+    <row r="494" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A494" s="2" t="s">
         <v>1190</v>
       </c>
@@ -24743,7 +24768,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="495" spans="1:13">
+    <row r="495" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A495" s="2" t="s">
         <v>971</v>
       </c>
@@ -24778,7 +24803,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="496" spans="1:13">
+    <row r="496" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A496" s="2" t="s">
         <v>973</v>
       </c>
@@ -24813,7 +24838,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="497" spans="1:13">
+    <row r="497" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A497" s="2" t="s">
         <v>809</v>
       </c>
@@ -24846,7 +24871,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="498" spans="1:13">
+    <row r="498" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A498" s="2" t="s">
         <v>1044</v>
       </c>
@@ -24879,7 +24904,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="499" spans="1:13">
+    <row r="499" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A499" s="2" t="s">
         <v>175</v>
       </c>
@@ -24916,7 +24941,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="500" spans="1:13">
+    <row r="500" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A500" s="2" t="s">
         <v>1195</v>
       </c>
@@ -24953,7 +24978,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="501" spans="1:13">
+    <row r="501" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A501" s="2" t="s">
         <v>950</v>
       </c>
@@ -24990,7 +25015,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="502" spans="1:13">
+    <row r="502" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A502" s="2" t="s">
         <v>948</v>
       </c>
@@ -25027,7 +25052,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="503" spans="1:13">
+    <row r="503" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A503" s="2" t="s">
         <v>211</v>
       </c>
@@ -25063,7 +25088,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="504" spans="1:13">
+    <row r="504" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A504" s="2" t="s">
         <v>131</v>
       </c>
@@ -25101,7 +25126,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="505" spans="1:13">
+    <row r="505" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A505" s="2" t="s">
         <v>55</v>
       </c>
@@ -25139,7 +25164,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="506" spans="1:13">
+    <row r="506" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A506" s="1" t="s">
         <v>237</v>
       </c>
@@ -25177,7 +25202,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="507" spans="1:13">
+    <row r="507" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A507" s="1" t="s">
         <v>186</v>
       </c>
@@ -25215,7 +25240,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="508" spans="1:13">
+    <row r="508" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A508" s="2" t="s">
         <v>1175</v>
       </c>
@@ -25252,7 +25277,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="509" spans="1:13">
+    <row r="509" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A509" s="2" t="s">
         <v>1192</v>
       </c>
@@ -25289,7 +25314,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="510" spans="1:13">
+    <row r="510" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A510" s="2" t="s">
         <v>1187</v>
       </c>
@@ -25326,7 +25351,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="511" spans="1:13">
+    <row r="511" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A511" s="2" t="s">
         <v>942</v>
       </c>
@@ -25363,7 +25388,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="512" spans="1:13">
+    <row r="512" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A512" s="2" t="s">
         <v>946</v>
       </c>
@@ -25400,7 +25425,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="513" spans="1:13">
+    <row r="513" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A513" s="2" t="s">
         <v>1224</v>
       </c>
@@ -25441,7 +25466,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="514" spans="1:13">
+    <row r="514" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A514" s="2" t="s">
         <v>212</v>
       </c>
@@ -25463,11 +25488,11 @@
       <c r="G514" s="2">
         <v>2005</v>
       </c>
-      <c r="H514" s="6" t="s">
-        <v>1150</v>
-      </c>
-      <c r="I514" s="6" t="s">
-        <v>1150</v>
+      <c r="H514" s="19" t="s">
+        <v>1327</v>
+      </c>
+      <c r="I514" s="19" t="s">
+        <v>1363</v>
       </c>
       <c r="J514" s="2" t="s">
         <v>1105</v>
@@ -25616,10 +25641,5 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>